<commit_message>
Change crowding parameter in downstairs flow function
</commit_message>
<xml_diff>
--- a/vce-onetrain/penn_station_platforms_20221109.xlsx
+++ b/vce-onetrain/penn_station_platforms_20221109.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\transit-modeling\vce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert_hale/transit-modeling/vce-onetrain/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C30D16-0E27-4594-8DDA-466B83245C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628A0A7A-831F-7242-A852-D535D156154F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="3015" windowWidth="20985" windowHeight="9525" xr2:uid="{A3B3AB15-1C45-5C4F-802C-007851D814A4}"/>
+    <workbookView xWindow="6680" yWindow="3020" windowWidth="20980" windowHeight="9520" xr2:uid="{A3B3AB15-1C45-5C4F-802C-007851D814A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -195,9 +199,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -235,7 +239,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -341,7 +345,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -483,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -493,13 +497,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4183AC29-8E9D-C649-AE42-B7CF346BD6A3}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +520,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -552,7 +556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -590,7 +594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -631,7 +635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -647,128 +651,128 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="1">
-        <v>60</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="H6" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="I6" s="1">
-        <v>60</v>
-      </c>
-      <c r="J6" s="1">
-        <v>60</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="H7" s="1">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="I7" s="1">
-        <v>60</v>
-      </c>
-      <c r="J7" s="1">
-        <v>60</v>
-      </c>
-      <c r="K7" s="1">
-        <v>60</v>
-      </c>
-      <c r="L7" s="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="1">
+        <v>60</v>
+      </c>
       <c r="E8" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G8" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="H8" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="I8" s="1">
-        <v>36</v>
-      </c>
-      <c r="J8" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="J8" s="1">
+        <v>60</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="N8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G9" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="I9" s="1">
-        <v>36</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="J9" s="1">
+        <v>60</v>
+      </c>
+      <c r="K9" s="1">
+        <v>60</v>
+      </c>
+      <c r="L9" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1">
         <v>60</v>
@@ -804,7 +808,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1">
         <v>40</v>
@@ -840,7 +844,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1">
         <v>58</v>
@@ -876,7 +880,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1">
         <v>57</v>
@@ -912,7 +916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="1">
         <v>57</v>
@@ -948,7 +952,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>57</v>
@@ -984,7 +988,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="1">
         <v>46</v>
@@ -1020,7 +1024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="1">
         <v>57</v>
@@ -1054,7 +1058,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="1">
         <v>46</v>
@@ -1080,21 +1084,21 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
       <c r="B21">
-        <f>SUM(B6:B20)</f>
+        <f t="shared" ref="B21:F21" si="0">SUM(B6:B20)</f>
         <v>530</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:L21" si="0">SUM(C6:C20)</f>
+        <f t="shared" si="0"/>
         <v>533</v>
       </c>
       <c r="D21">
@@ -1110,51 +1114,80 @@
         <v>678</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f>SUM(G6:G20)</f>
         <v>650</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H21:L21" si="1">SUM(H6:H20)</f>
         <v>625</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>625</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>582</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>828</v>
       </c>
       <c r="L21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>636</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="1">
-        <v>450</v>
+      <c r="B22">
+        <f t="shared" ref="B22:F22" si="2">SUM(B8:B20)</f>
+        <v>530</v>
       </c>
       <c r="C22">
-        <v>450</v>
+        <f t="shared" si="2"/>
+        <v>533</v>
       </c>
       <c r="D22">
-        <v>500</v>
+        <f t="shared" si="2"/>
+        <v>537</v>
       </c>
       <c r="E22">
-        <v>550</v>
+        <f t="shared" si="2"/>
+        <v>614</v>
       </c>
       <c r="F22">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>606</v>
+      </c>
+      <c r="G22">
+        <f>SUM(G8:G20)</f>
+        <v>578</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22:L22" si="3">SUM(H8:H20)</f>
+        <v>553</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>553</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>582</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>828</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>636</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>8</v>
       </c>
@@ -1189,12 +1222,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>22</v>
       </c>
@@ -1205,7 +1238,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>17</v>
       </c>
@@ -1213,17 +1246,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>25</v>
       </c>

</xml_diff>